<commit_message>
20250410 until Liq constraints
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202504/Developed Market.xlsx
+++ b/GUI + Reviews/202504/Developed Market.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FF0EBC4F-87FA-4880-ABDF-10E9D1B9D9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DE207F1-2057-4C7B-B5C8-B650127E33B1}"/>
   <bookViews>
-    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15840" xr2:uid="{55E1B219-E43B-4FF8-A49F-37EA82F17A1F}"/>
+    <workbookView xWindow="-315" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{55E1B219-E43B-4FF8-A49F-37EA82F17A1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14714,8 +14714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DBDFA6-8ACF-46B1-986C-8B78F48A2240}">
   <dimension ref="A1:K1547"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1101" workbookViewId="0">
-      <selection activeCell="G1120" sqref="G1120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>